<commit_message>
Update DMA register table, including full names
</commit_message>
<xml_diff>
--- a/teensy_minimal_rpc/notebooks/register-field-descriptions.xlsx
+++ b/teensy_minimal_rpc/notebooks/register-field-descriptions.xlsx
@@ -5,19 +5,19 @@
   <workbookPr checkCompatibility="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\teensy-minimal-rpc\teensy_minimal_rpc\notebooks\dma-examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\teensy-minimal-rpc\teensy_minimal_rpc\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5952" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5952" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="dma" sheetId="1" r:id="rId1"/>
-    <sheet name="sim" sheetId="2" r:id="rId2"/>
-    <sheet name="adc" sheetId="3" r:id="rId3"/>
+    <sheet name="dma mem map" sheetId="1" r:id="rId1"/>
+    <sheet name="dma registers" sheetId="4" r:id="rId2"/>
+    <sheet name="sim" sheetId="2" r:id="rId3"/>
+    <sheet name="adc" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="553">
   <si>
     <t>4000_8000</t>
   </si>
@@ -644,9 +644,6 @@
     <t>Channel priority when fixed-priority arbitration is enabled.  NOTE: Reset value for the channel priority fields, CHPRI, is equal to the corresponding channel number for each priority register, i.e., DCHPRI15[CHPRI] equals 0b1111.</t>
   </si>
   <si>
-    <t>TCD_ATTR</t>
-  </si>
-  <si>
     <t>SMOD</t>
   </si>
   <si>
@@ -680,9 +677,6 @@
     <t>Destination data transfer size</t>
   </si>
   <si>
-    <t>TCD_NBYTES_MLNO</t>
-  </si>
-  <si>
     <t>NBYTES</t>
   </si>
   <si>
@@ -692,9 +686,6 @@
     <t>Number of bytes to be transferred in each service request of the channel. As a channel activates, the appropriate TCD contents load into the eDMA engine, and the appropriate reads and writes perform until the minor byte transfer count has transferred. This is an indivisible operation and cannot be halted. (Although, it may be stalled by using the bandwidth control field, or via preemption.) After the minor count is exhausted, the SADDR and DADDR values are written back into the TCD memory, the major iteration count is decremented and restored to the TCD memory. If the major iteration count is completed, additional processing is performed. NOTE: An NBYTES value of 0x0000_0000 is interpreted as a 4 GB transfer.</t>
   </si>
   <si>
-    <t>TCD_NBYTES_MLOFFNO</t>
-  </si>
-  <si>
     <t>SMLOE</t>
   </si>
   <si>
@@ -716,9 +707,6 @@
     <t>Number of bytes to be transferred in each service request of the channel. As a channel activates, the appropriate TCD contents load into the eDMA engine, and the appropriate reads and writes perform until the minor byte transfer count has transferred. This is an indivisible operation and cannot be halted; although, it may be stalled by using the bandwidth control field, or via preemption. After the minor count is exhausted, the SADDR and DADDR values are written back into the TCD memory, the major iteration count is decremented and restored to the TCD memory. If the major iteration count is completed, additional processing is performed.</t>
   </si>
   <si>
-    <t>TCD_NBYTES_MLOFFYES</t>
-  </si>
-  <si>
     <t>MLOFF</t>
   </si>
   <si>
@@ -728,18 +716,12 @@
     <t>Minor Loop Offset</t>
   </si>
   <si>
-    <t>TCD_SLAST</t>
-  </si>
-  <si>
     <t>SLAST</t>
   </si>
   <si>
     <t>Last source Address Adjustment</t>
   </si>
   <si>
-    <t>TCD_DADDR</t>
-  </si>
-  <si>
     <t>DADDR</t>
   </si>
   <si>
@@ -761,12 +743,6 @@
     <t>Sign-extended offset applied to the current destination address to form the next-state value as each destination write is completed.</t>
   </si>
   <si>
-    <t>TCD_DOFF</t>
-  </si>
-  <si>
-    <t>TCD_CITER_ELINKYES</t>
-  </si>
-  <si>
     <t>ELINK</t>
   </si>
   <si>
@@ -785,24 +761,15 @@
     <t>If channel-to-channel linking is enabled (ELINK = 1), then after the minor loop is exhausted, the eDMA engine initiates a channel service request to the channel defined by these four bits by setting that channel’s TCDn_CSR[START] bit.</t>
   </si>
   <si>
-    <t>CITER</t>
-  </si>
-  <si>
     <t>Current Major Iteration Count</t>
   </si>
   <si>
     <t>This 9-bit (ELINK = 1) or 15-bit (ELINK = 0) count represents the current major loop count for the channel. It is decremented each time the minor loop is completed and updated in the transfer control descriptor memory. After the major iteration count is exhausted, the channel performs a number of operations (e.g., final source and destination address calculations), optionally generating an interrupt to signal channel completion before reloading the CITER field from the beginning iteration count (BITER) field. NOTE: When the CITER field is initially loaded by software, it must be set to the same value as that contained in the BITER field. NOTE: If the channel is configured to execute a single service request, the initial values of BITER and CITER should be 0x0001.</t>
   </si>
   <si>
-    <t>TCD_CITER_ELINKNO</t>
-  </si>
-  <si>
     <t>This 9-bit (ELINK = 1) or 15-bit (ELINK = 0) count represents the current major loop count for the channel. It is decremented each time the minor loop is completed and updated in the transfer control descriptor memory. After the major iteration count is exhausted, the channel performs a number of operations (e.g., final source and destination address calculations), optionally generating an interrupt to signal channel completion before reloading the CITER field from the beginning iteration count (BITER) field. NOTE: When the CITER field is initially loaded by software, it must be set to the same value as that contained in the BITER field. NOTE: If the channel is configured to execute a single service request, the initial values of BITER and CITER should be 0x0001.E87</t>
   </si>
   <si>
-    <t>TCD_DLASTSGA</t>
-  </si>
-  <si>
     <t>DLASTSGA</t>
   </si>
   <si>
@@ -812,9 +779,6 @@
     <t>If (TCDn_CSR[ESG] = 0) then adjustment value added to the destination address at the completion of the major iteration count. This value can apply to restore the destination address to the initial value or adjust the address to reference the next data structure. Otherwise, this address points to the beginning of a 0-modulo-32-byte region containing the next transfer control descriptor to be loaded into this channel. This channel reload is performed as the major iteration count completes. The scatter/gather address must be 0-modulo-32-byte, else a configuration error is reported.eference the next data structure.</t>
   </si>
   <si>
-    <t>TCD_CSR</t>
-  </si>
-  <si>
     <t>BWC</t>
   </si>
   <si>
@@ -902,15 +866,6 @@
     <t>If this flag is set, the channel is requesting service. The eDMA hardware automatically clears this flag after the channel begins execution. 0: The channel is not explicitly started, 1: The channel is explicitly started via a software initiated service request,</t>
   </si>
   <si>
-    <t>TCD_BITER_ELINKYES</t>
-  </si>
-  <si>
-    <t>BITER</t>
-  </si>
-  <si>
-    <t>TCD_BITER_ELINKNO</t>
-  </si>
-  <si>
     <t>See CITER_ELINKYES[ELINK].</t>
   </si>
   <si>
@@ -929,9 +884,6 @@
     <t>Structs</t>
   </si>
   <si>
-    <t>TCD_SADDR</t>
-  </si>
-  <si>
     <t>SADDR</t>
   </si>
   <si>
@@ -941,9 +893,6 @@
     <t>Memory address pointing to the source data.</t>
   </si>
   <si>
-    <t>TCD_SOFF</t>
-  </si>
-  <si>
     <t>SOFF</t>
   </si>
   <si>
@@ -1695,6 +1644,48 @@
   </si>
   <si>
     <t>Compare function enable</t>
+  </si>
+  <si>
+    <t>Parent register</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Full name</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>NBYTES_MLNO</t>
+  </si>
+  <si>
+    <t>ATTR</t>
+  </si>
+  <si>
+    <t>NBYTES_MLOFFNO</t>
+  </si>
+  <si>
+    <t>NBYTES_MLOFFYES</t>
+  </si>
+  <si>
+    <t>CITER_ELINKYES</t>
+  </si>
+  <si>
+    <t>CITER_ELINKNO</t>
+  </si>
+  <si>
+    <t>CSR</t>
+  </si>
+  <si>
+    <t>BITER_ELINKYES</t>
+  </si>
+  <si>
+    <t>BITER_ELINKNO</t>
+  </si>
+  <si>
+    <t>ITER</t>
   </si>
 </sst>
 </file>
@@ -2012,9 +2003,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:G116"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2927,1101 +2920,1516 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" t="s">
-        <v>125</v>
-      </c>
-      <c r="D47" t="s">
-        <v>126</v>
-      </c>
-      <c r="E47" t="str">
-        <f>"  optional " &amp; IF(B47&gt;0,"uint32", "bool") &amp; " " &amp; C47 &amp; " = 1; // " &amp; D47</f>
-        <v xml:space="preserve">  optional bool CX = 1; // Cancel Transfer</v>
-      </c>
-      <c r="F47" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
-        <v>127</v>
-      </c>
-      <c r="D48" t="s">
-        <v>128</v>
-      </c>
-      <c r="E48" t="str">
-        <f t="shared" ref="E48:E66" si="0">"  optional " &amp; IF(B48&gt;0,"uint32", "bool") &amp; " " &amp; C48 &amp; " = 1; // " &amp; D48</f>
-        <v xml:space="preserve">  optional bool ECX = 1; // Error Cancel Transfer</v>
-      </c>
-      <c r="F48" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
-        <v>131</v>
-      </c>
-      <c r="D49" t="s">
-        <v>133</v>
-      </c>
-      <c r="E49" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool EMLM = 1; // Enable Minor Loop Mapping</v>
-      </c>
-      <c r="F49" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
-        <v>134</v>
-      </c>
-      <c r="D50" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool CLM = 1; // Continuous Link Mode</v>
-      </c>
-      <c r="F50" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
-        <v>137</v>
-      </c>
-      <c r="D51" t="s">
-        <v>138</v>
-      </c>
-      <c r="E51" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool HALT = 1; // Halt DMA Operations</v>
-      </c>
-      <c r="F51" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>140</v>
-      </c>
-      <c r="D52" t="s">
-        <v>141</v>
-      </c>
-      <c r="E52" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool HOE = 1; // Halt On Error</v>
-      </c>
-      <c r="F52" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>143</v>
-      </c>
-      <c r="D53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E53" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool ERCA = 1; // Enable Round Robin Channel Arbitration</v>
-      </c>
-      <c r="F53" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>146</v>
-      </c>
-      <c r="D54" t="s">
-        <v>147</v>
-      </c>
-      <c r="E54" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool EDBG = 1; // Enable Debug</v>
-      </c>
-      <c r="F54" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>149</v>
-      </c>
-      <c r="C55" t="s">
-        <v>150</v>
-      </c>
-      <c r="D55" t="s">
-        <v>151</v>
-      </c>
-      <c r="E55" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool VLD = 1; // Logical OR of all ERR status bits</v>
-      </c>
-      <c r="F55" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
-        <v>127</v>
-      </c>
-      <c r="D56" t="s">
-        <v>153</v>
-      </c>
-      <c r="E56" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool ECX = 1; // Transfer Cancelled</v>
-      </c>
-      <c r="F56" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>155</v>
-      </c>
-      <c r="D57" t="s">
-        <v>156</v>
-      </c>
-      <c r="E57" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool CPE = 1; // Channel Priority Error</v>
-      </c>
-      <c r="F57" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B58">
-        <v>4</v>
-      </c>
-      <c r="C58" t="s">
-        <v>158</v>
-      </c>
-      <c r="D58" t="s">
-        <v>159</v>
-      </c>
-      <c r="E58" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional uint32 ERRCHN = 1; // Error Channel Number or Cancelled Channel Number</v>
-      </c>
-      <c r="F58" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
-        <v>161</v>
-      </c>
-      <c r="D59" t="s">
-        <v>162</v>
-      </c>
-      <c r="E59" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool SAE = 1; // Source Address Error</v>
-      </c>
-      <c r="F59" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
-        <v>164</v>
-      </c>
-      <c r="D60" t="s">
-        <v>165</v>
-      </c>
-      <c r="E60" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool SOE = 1; // Source Offset Error</v>
-      </c>
-      <c r="F60" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C61" t="s">
-        <v>167</v>
-      </c>
-      <c r="D61" t="s">
-        <v>168</v>
-      </c>
-      <c r="E61" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool DAE = 1; // Destination Address Error</v>
-      </c>
-      <c r="F61" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
-        <v>170</v>
-      </c>
-      <c r="D62" t="s">
-        <v>171</v>
-      </c>
-      <c r="E62" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool DOE = 1; // Destination Offset Error</v>
-      </c>
-      <c r="F62" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
-        <v>173</v>
-      </c>
-      <c r="D63" t="s">
-        <v>174</v>
-      </c>
-      <c r="E63" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool NCE = 1; // NBYTES/CITER Configuration Error</v>
-      </c>
-      <c r="F63" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
-        <v>176</v>
-      </c>
-      <c r="D64" t="s">
-        <v>177</v>
-      </c>
-      <c r="E64" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool SGE = 1; // Scatter/Gather Configuration Error</v>
-      </c>
-      <c r="F64" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
-        <v>179</v>
-      </c>
-      <c r="D65" t="s">
-        <v>180</v>
-      </c>
-      <c r="E65" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool SBE = 1; // Source Bus Error</v>
-      </c>
-      <c r="F65" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>182</v>
-      </c>
-      <c r="D66" t="s">
-        <v>183</v>
-      </c>
-      <c r="E66" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  optional bool DBE = 1; // Destination Bus Error</v>
-      </c>
-      <c r="F66" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>185</v>
-      </c>
-      <c r="B67">
-        <v>16</v>
-      </c>
-      <c r="D67" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>187</v>
-      </c>
-      <c r="B68">
-        <v>16</v>
-      </c>
-      <c r="D68" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>189</v>
-      </c>
-      <c r="B69">
-        <v>16</v>
-      </c>
-      <c r="D69" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>191</v>
-      </c>
-      <c r="B70">
-        <v>16</v>
-      </c>
-      <c r="D70" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>193</v>
-      </c>
-      <c r="B71">
-        <v>16</v>
-      </c>
-      <c r="D71" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>195</v>
-      </c>
-      <c r="C75" t="s">
-        <v>196</v>
-      </c>
-      <c r="D75" t="s">
-        <v>197</v>
-      </c>
-      <c r="E75" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C76" t="s">
-        <v>199</v>
-      </c>
-      <c r="D76" t="s">
-        <v>200</v>
-      </c>
-      <c r="E76" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B77">
-        <v>4</v>
-      </c>
-      <c r="C77" t="s">
-        <v>202</v>
-      </c>
-      <c r="D77" t="s">
-        <v>203</v>
-      </c>
-      <c r="E77" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>300</v>
-      </c>
-      <c r="B79">
-        <v>32</v>
-      </c>
-      <c r="C79" t="s">
-        <v>301</v>
-      </c>
-      <c r="D79" t="s">
-        <v>302</v>
-      </c>
-      <c r="E79" t="str">
-        <f>"  optional " &amp; IF(B79&gt;0,"uint32", "bool") &amp; " " &amp; C79 &amp; " = 1; // " &amp; D79</f>
-        <v xml:space="preserve">  optional uint32 SADDR = 1; // Source Address</v>
-      </c>
-      <c r="F79" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>304</v>
-      </c>
-      <c r="B80">
-        <v>16</v>
-      </c>
-      <c r="C80" t="s">
-        <v>305</v>
-      </c>
-      <c r="D80" t="s">
-        <v>306</v>
-      </c>
-      <c r="E80" t="str">
-        <f t="shared" ref="E80:E116" si="1">"  optional " &amp; IF(B80&gt;0,"uint32", "bool") &amp; " " &amp; C80 &amp; " = 1; // " &amp; D80</f>
-        <v xml:space="preserve">  optional uint32 SOFF = 1; // Source Address Signed offset</v>
-      </c>
-      <c r="F80" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>205</v>
-      </c>
-      <c r="B81">
-        <v>5</v>
-      </c>
-      <c r="C81" t="s">
-        <v>206</v>
-      </c>
-      <c r="D81" t="s">
-        <v>207</v>
-      </c>
-      <c r="E81" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 SMOD = 1; // Source Address Modulo.</v>
-      </c>
-      <c r="F81" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B82">
-        <v>3</v>
-      </c>
-      <c r="C82" t="s">
-        <v>209</v>
-      </c>
-      <c r="D82" t="s">
-        <v>210</v>
-      </c>
-      <c r="E82" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 SSIZE = 1; // Source data transfer size</v>
-      </c>
-      <c r="F82" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B83">
-        <v>5</v>
-      </c>
-      <c r="C83" t="s">
-        <v>212</v>
-      </c>
-      <c r="D83" t="s">
-        <v>213</v>
-      </c>
-      <c r="E83" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 DMOD = 1; // Destination Address Modulo</v>
-      </c>
-      <c r="F83" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B84">
-        <v>3</v>
-      </c>
-      <c r="C84" t="s">
-        <v>215</v>
-      </c>
-      <c r="D84" t="s">
-        <v>216</v>
-      </c>
-      <c r="E84" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 DSIZE = 1; // Destination data transfer size</v>
-      </c>
-      <c r="F84" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>217</v>
-      </c>
-      <c r="B85">
-        <v>32</v>
-      </c>
-      <c r="C85" t="s">
-        <v>218</v>
-      </c>
-      <c r="D85" t="s">
-        <v>219</v>
-      </c>
-      <c r="E85" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 NBYTES = 1; // Minor Byte Transfer Count</v>
-      </c>
-      <c r="F85" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>221</v>
-      </c>
-      <c r="C86" t="s">
-        <v>222</v>
-      </c>
-      <c r="D86" t="s">
-        <v>223</v>
-      </c>
-      <c r="E86" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool SMLOE = 1; // Source Minor Loop Offset Enable</v>
-      </c>
-      <c r="F86" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C87" t="s">
-        <v>225</v>
-      </c>
-      <c r="D87" t="s">
-        <v>226</v>
-      </c>
-      <c r="E87" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool DMLOE = 1; // Destination Minor Loop Offset enable</v>
-      </c>
-      <c r="F87" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B88">
-        <v>30</v>
-      </c>
-      <c r="C88" t="s">
-        <v>218</v>
-      </c>
-      <c r="D88" t="s">
-        <v>219</v>
-      </c>
-      <c r="E88" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 NBYTES = 1; // Minor Byte Transfer Count</v>
-      </c>
-      <c r="F88" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>229</v>
-      </c>
-      <c r="C89" t="s">
-        <v>222</v>
-      </c>
-      <c r="D89" t="s">
-        <v>223</v>
-      </c>
-      <c r="E89" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool SMLOE = 1; // Source Minor Loop Offset Enable</v>
-      </c>
-      <c r="F89" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C90" t="s">
-        <v>225</v>
-      </c>
-      <c r="D90" t="s">
-        <v>226</v>
-      </c>
-      <c r="E90" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool DMLOE = 1; // Destination Minor Loop Offset enable</v>
-      </c>
-      <c r="F90" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B91">
-        <v>20</v>
-      </c>
-      <c r="C91" t="s">
-        <v>230</v>
-      </c>
-      <c r="D91" t="s">
-        <v>232</v>
-      </c>
-      <c r="E91" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 MLOFF = 1; // Minor Loop Offset</v>
-      </c>
-      <c r="F91" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B92">
-        <v>10</v>
-      </c>
-      <c r="C92" t="s">
-        <v>218</v>
-      </c>
-      <c r="D92" t="s">
-        <v>219</v>
-      </c>
-      <c r="E92" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 NBYTES = 1; // Minor Byte Transfer Count</v>
-      </c>
-      <c r="F92" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>233</v>
-      </c>
-      <c r="B93">
-        <v>32</v>
-      </c>
-      <c r="C93" t="s">
-        <v>234</v>
-      </c>
-      <c r="D93" t="s">
-        <v>235</v>
-      </c>
-      <c r="E93" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 SLAST = 1; // Last source Address Adjustment</v>
-      </c>
-      <c r="F93" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>236</v>
-      </c>
-      <c r="B94">
-        <v>32</v>
-      </c>
-      <c r="C94" t="s">
-        <v>237</v>
-      </c>
-      <c r="D94" t="s">
-        <v>238</v>
-      </c>
-      <c r="E94" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 DADDR = 1; // Destination Address</v>
-      </c>
-      <c r="F94" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>244</v>
-      </c>
-      <c r="B95">
-        <v>16</v>
-      </c>
-      <c r="C95" t="s">
-        <v>241</v>
-      </c>
-      <c r="D95" t="s">
-        <v>242</v>
-      </c>
-      <c r="E95" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 DOFF = 1; // Destination Address Signed offset</v>
-      </c>
-      <c r="F95" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>245</v>
-      </c>
-      <c r="C96" t="s">
-        <v>246</v>
-      </c>
-      <c r="D96" t="s">
-        <v>247</v>
-      </c>
-      <c r="E96" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool ELINK = 1; // Enable channel-to-channel linking on minor-loop complete</v>
-      </c>
-      <c r="F96" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B97">
-        <v>4</v>
-      </c>
-      <c r="C97" t="s">
-        <v>249</v>
-      </c>
-      <c r="D97" t="s">
-        <v>250</v>
-      </c>
-      <c r="E97" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 LINKCH = 1; // Link Channel Number</v>
-      </c>
-      <c r="F97" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B98">
-        <v>9</v>
-      </c>
-      <c r="C98" t="s">
-        <v>252</v>
-      </c>
-      <c r="D98" t="s">
-        <v>253</v>
-      </c>
-      <c r="E98" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 CITER = 1; // Current Major Iteration Count</v>
-      </c>
-      <c r="F98" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>255</v>
-      </c>
-      <c r="C99" t="s">
-        <v>246</v>
-      </c>
-      <c r="D99" t="s">
-        <v>247</v>
-      </c>
-      <c r="E99" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool ELINK = 1; // Enable channel-to-channel linking on minor-loop complete</v>
-      </c>
-      <c r="F99" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B100">
-        <v>15</v>
-      </c>
-      <c r="C100" t="s">
-        <v>252</v>
-      </c>
-      <c r="D100" t="s">
-        <v>253</v>
-      </c>
-      <c r="E100" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 CITER = 1; // Current Major Iteration Count</v>
-      </c>
-      <c r="F100" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>257</v>
-      </c>
-      <c r="B101">
-        <v>32</v>
-      </c>
-      <c r="C101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" t="s">
-        <v>259</v>
-      </c>
-      <c r="E101" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 DLASTSGA = 1; // Destination last address adjustment or the memory address for the next transfer control descriptor to be loaded into this channel (scatter/gather).</v>
-      </c>
-      <c r="F101" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>261</v>
-      </c>
-      <c r="B102">
-        <v>2</v>
-      </c>
-      <c r="C102" t="s">
-        <v>262</v>
-      </c>
-      <c r="D102" t="s">
-        <v>263</v>
-      </c>
-      <c r="E102" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 BWC = 1; // Bandwidth Control</v>
-      </c>
-      <c r="F102" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B103">
-        <v>4</v>
-      </c>
-      <c r="C103" t="s">
-        <v>265</v>
-      </c>
-      <c r="D103" t="s">
-        <v>250</v>
-      </c>
-      <c r="E103" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 MAJORLINKCH = 1; // Link Channel Number</v>
-      </c>
-      <c r="F103" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C104" t="s">
-        <v>267</v>
-      </c>
-      <c r="D104" t="s">
-        <v>268</v>
-      </c>
-      <c r="E104" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool DONE = 1; // Channel Done</v>
-      </c>
-      <c r="F104" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C105" t="s">
-        <v>270</v>
-      </c>
-      <c r="D105" t="s">
-        <v>271</v>
-      </c>
-      <c r="E105" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool ACTIVE = 1; // Channel Active</v>
-      </c>
-      <c r="F105" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C106" t="s">
-        <v>273</v>
-      </c>
-      <c r="D106" t="s">
-        <v>274</v>
-      </c>
-      <c r="E106" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool MAJORELINK = 1; // Enable channel-to-channel linking on major loop complete</v>
-      </c>
-      <c r="F106" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C107" t="s">
-        <v>276</v>
-      </c>
-      <c r="D107" t="s">
-        <v>277</v>
-      </c>
-      <c r="E107" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool ESG = 1; // Enable Scatter/Gather Processing</v>
-      </c>
-      <c r="F107" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C108" t="s">
-        <v>279</v>
-      </c>
-      <c r="D108" t="s">
-        <v>280</v>
-      </c>
-      <c r="E108" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool DREQ = 1; // Disable Request</v>
-      </c>
-      <c r="F108" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C109" t="s">
-        <v>282</v>
-      </c>
-      <c r="D109" t="s">
-        <v>283</v>
-      </c>
-      <c r="E109" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool INTHALF = 1; // Enable an interrupt when major counter is half complete.</v>
-      </c>
-      <c r="F109" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C110" t="s">
-        <v>285</v>
-      </c>
-      <c r="D110" t="s">
-        <v>286</v>
-      </c>
-      <c r="E110" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool INTMAJOR = 1; // Enable an interrupt when major iteration count completes</v>
-      </c>
-      <c r="F110" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C111" t="s">
-        <v>288</v>
-      </c>
-      <c r="D111" t="s">
-        <v>289</v>
-      </c>
-      <c r="E111" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool START = 1; // Channel Start</v>
-      </c>
-      <c r="F111" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>291</v>
-      </c>
-      <c r="C112" t="s">
-        <v>246</v>
-      </c>
-      <c r="D112" t="s">
-        <v>247</v>
-      </c>
-      <c r="E112" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool ELINK = 1; // Enable channel-to-channel linking on minor-loop complete</v>
-      </c>
-      <c r="F112" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B113">
-        <v>4</v>
-      </c>
-      <c r="C113" t="s">
-        <v>249</v>
-      </c>
-      <c r="D113" t="s">
-        <v>250</v>
-      </c>
-      <c r="E113" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 LINKCH = 1; // Link Channel Number</v>
-      </c>
-      <c r="F113" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B114">
-        <v>9</v>
-      </c>
-      <c r="C114" t="s">
-        <v>292</v>
-      </c>
-      <c r="D114" t="s">
-        <v>253</v>
-      </c>
-      <c r="E114" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 BITER = 1; // Current Major Iteration Count</v>
-      </c>
-      <c r="F114" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>293</v>
-      </c>
-      <c r="C115" t="s">
-        <v>246</v>
-      </c>
-      <c r="D115" t="s">
-        <v>247</v>
-      </c>
-      <c r="E115" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional bool ELINK = 1; // Enable channel-to-channel linking on minor-loop complete</v>
-      </c>
-      <c r="F115" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B116">
-        <v>15</v>
-      </c>
-      <c r="C116" t="s">
-        <v>292</v>
-      </c>
-      <c r="D116" t="s">
-        <v>253</v>
-      </c>
-      <c r="E116" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  optional uint32 BITER = 1; // Current Major Iteration Count</v>
-      </c>
-      <c r="F116" t="s">
-        <v>298</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.21875" customWidth="1"/>
+    <col min="7" max="7" width="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D1" t="s">
+        <v>540</v>
+      </c>
+      <c r="E1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="str">
+        <f>B$2&amp;"."&amp;D2</f>
+        <v>CR.CX</v>
+      </c>
+      <c r="F2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G9" si="0">"  optional " &amp; IF(C2&gt;0,"uint32", "bool") &amp; " " &amp; D2 &amp; " = "&amp;A2&amp;"; // " &amp; F2</f>
+        <v xml:space="preserve">  optional bool CX = 1; // Cancel Transfer</v>
+      </c>
+      <c r="H2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E10" si="1">B$2&amp;"."&amp;D3</f>
+        <v>CR.ECX</v>
+      </c>
+      <c r="F3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  optional bool ECX = 2; // Error Cancel Transfer</v>
+      </c>
+      <c r="H3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>CR.EMLM</v>
+      </c>
+      <c r="F4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  optional bool EMLM = 3; // Enable Minor Loop Mapping</v>
+      </c>
+      <c r="H4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>CR.CLM</v>
+      </c>
+      <c r="F5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  optional bool CLM = 4; // Continuous Link Mode</v>
+      </c>
+      <c r="H5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>CR.HALT</v>
+      </c>
+      <c r="F6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  optional bool HALT = 5; // Halt DMA Operations</v>
+      </c>
+      <c r="H6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>CR.HOE</v>
+      </c>
+      <c r="F7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  optional bool HOE = 6; // Halt On Error</v>
+      </c>
+      <c r="H7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>CR.ERCA</v>
+      </c>
+      <c r="F8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  optional bool ERCA = 7; // Enable Round Robin Channel Arbitration</v>
+      </c>
+      <c r="H8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>CR.EDBG</v>
+      </c>
+      <c r="F9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  optional bool EDBG = 8; // Enable Debug</v>
+      </c>
+      <c r="H9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" t="str">
+        <f>B$10&amp;"."&amp;D10</f>
+        <v>ES.VLD</v>
+      </c>
+      <c r="F10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" t="str">
+        <f>"  optional " &amp; IF(C10&gt;0,"uint32", "bool") &amp; " " &amp; D10 &amp; " = "&amp;A10&amp;"; // " &amp; F10</f>
+        <v xml:space="preserve">  optional bool VLD = 1; // Logical OR of all ERR status bits</v>
+      </c>
+      <c r="H10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" ref="E11:E21" si="2">B$10&amp;"."&amp;D11</f>
+        <v>ES.ECX</v>
+      </c>
+      <c r="F11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" ref="G11:G21" si="3">"  optional " &amp; IF(C11&gt;0,"uint32", "bool") &amp; " " &amp; D11 &amp; " = "&amp;A11&amp;"; // " &amp; F11</f>
+        <v xml:space="preserve">  optional bool ECX = 2; // Transfer Cancelled</v>
+      </c>
+      <c r="H11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.CPE</v>
+      </c>
+      <c r="F12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional bool CPE = 3; // Channel Priority Error</v>
+      </c>
+      <c r="H12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.ERRCHN</v>
+      </c>
+      <c r="F13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional uint32 ERRCHN = 4; // Error Channel Number or Cancelled Channel Number</v>
+      </c>
+      <c r="H13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.SAE</v>
+      </c>
+      <c r="F14" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional bool SAE = 5; // Source Address Error</v>
+      </c>
+      <c r="H14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.SOE</v>
+      </c>
+      <c r="F15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional bool SOE = 6; // Source Offset Error</v>
+      </c>
+      <c r="H15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.DAE</v>
+      </c>
+      <c r="F16" t="s">
+        <v>168</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional bool DAE = 7; // Destination Address Error</v>
+      </c>
+      <c r="H16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.DOE</v>
+      </c>
+      <c r="F17" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional bool DOE = 8; // Destination Offset Error</v>
+      </c>
+      <c r="H17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.NCE</v>
+      </c>
+      <c r="F18" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional bool NCE = 9; // NBYTES/CITER Configuration Error</v>
+      </c>
+      <c r="H18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>176</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.SGE</v>
+      </c>
+      <c r="F19" t="s">
+        <v>177</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional bool SGE = 10; // Scatter/Gather Configuration Error</v>
+      </c>
+      <c r="H19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.SBE</v>
+      </c>
+      <c r="F20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional bool SBE = 11; // Source Bus Error</v>
+      </c>
+      <c r="H20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>ES.DBE</v>
+      </c>
+      <c r="F21" t="s">
+        <v>183</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  optional bool DBE = 12; // Destination Bus Error</v>
+      </c>
+      <c r="H21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="E22" t="str">
+        <f>B22</f>
+        <v>ERQ</v>
+      </c>
+      <c r="F22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23">
+        <v>16</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" ref="E23:E26" si="4">B23</f>
+        <v>EEI</v>
+      </c>
+      <c r="F23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24">
+        <v>16</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="4"/>
+        <v>INT</v>
+      </c>
+      <c r="F24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>191</v>
+      </c>
+      <c r="C25">
+        <v>16</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="4"/>
+        <v>ERR</v>
+      </c>
+      <c r="F25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>193</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="4"/>
+        <v>HRS</v>
+      </c>
+      <c r="F26" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>284</v>
+      </c>
+      <c r="E29" t="s">
+        <v>430</v>
+      </c>
+      <c r="F29" t="s">
+        <v>431</v>
+      </c>
+      <c r="H29" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D30" t="s">
+        <v>196</v>
+      </c>
+      <c r="E30" t="str">
+        <f>B$30&amp;"."&amp;D30</f>
+        <v>DCHPRI.ECP</v>
+      </c>
+      <c r="F30" t="s">
+        <v>197</v>
+      </c>
+      <c r="H30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>199</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" ref="E31:E34" si="5">B$30&amp;"."&amp;D31</f>
+        <v>DCHPRI.DPA</v>
+      </c>
+      <c r="F31" t="s">
+        <v>200</v>
+      </c>
+      <c r="H31" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>202</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="5"/>
+        <v>DCHPRI.CHPRI</v>
+      </c>
+      <c r="F32" t="s">
+        <v>203</v>
+      </c>
+      <c r="H32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>285</v>
+      </c>
+      <c r="E34" t="str">
+        <f>D34</f>
+        <v>SADDR</v>
+      </c>
+      <c r="F34" t="s">
+        <v>286</v>
+      </c>
+      <c r="H34" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>288</v>
+      </c>
+      <c r="E35" t="str">
+        <f>D35</f>
+        <v>SOFF</v>
+      </c>
+      <c r="F35" t="s">
+        <v>289</v>
+      </c>
+      <c r="H35" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>544</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>205</v>
+      </c>
+      <c r="E36" t="str">
+        <f>B$36&amp;"."&amp;D36</f>
+        <v>ATTR.SMOD</v>
+      </c>
+      <c r="F36" t="s">
+        <v>206</v>
+      </c>
+      <c r="G36" t="str">
+        <f>"  optional " &amp; IF(C36&gt;0,"uint32", "bool") &amp; " " &amp; D36 &amp; " = "&amp;A36&amp;"; // " &amp; F36</f>
+        <v xml:space="preserve">  optional uint32 SMOD = 1; // Source Address Modulo.</v>
+      </c>
+      <c r="H36" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>208</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" ref="E37:E40" si="6">B$36&amp;"."&amp;D37</f>
+        <v>ATTR.SSIZE</v>
+      </c>
+      <c r="F37" t="s">
+        <v>209</v>
+      </c>
+      <c r="G37" t="str">
+        <f>"  optional " &amp; IF(C37&gt;0,"uint32", "bool") &amp; " " &amp; D37 &amp; " = "&amp;A37&amp;"; // " &amp; F37</f>
+        <v xml:space="preserve">  optional uint32 SSIZE = 2; // Source data transfer size</v>
+      </c>
+      <c r="H37" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>211</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="6"/>
+        <v>ATTR.DMOD</v>
+      </c>
+      <c r="F38" t="s">
+        <v>212</v>
+      </c>
+      <c r="G38" t="str">
+        <f>"  optional " &amp; IF(C38&gt;0,"uint32", "bool") &amp; " " &amp; D38 &amp; " = "&amp;A38&amp;"; // " &amp; F38</f>
+        <v xml:space="preserve">  optional uint32 DMOD = 3; // Destination Address Modulo</v>
+      </c>
+      <c r="H38" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>214</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="6"/>
+        <v>ATTR.DSIZE</v>
+      </c>
+      <c r="F39" t="s">
+        <v>215</v>
+      </c>
+      <c r="G39" t="str">
+        <f>"  optional " &amp; IF(C39&gt;0,"uint32", "bool") &amp; " " &amp; D39 &amp; " = "&amp;A39&amp;"; // " &amp; F39</f>
+        <v xml:space="preserve">  optional uint32 DSIZE = 4; // Destination data transfer size</v>
+      </c>
+      <c r="H39" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>32</v>
+      </c>
+      <c r="D40" t="s">
+        <v>543</v>
+      </c>
+      <c r="E40" t="str">
+        <f>D40</f>
+        <v>NBYTES_MLNO</v>
+      </c>
+      <c r="F40" t="s">
+        <v>217</v>
+      </c>
+      <c r="H40" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>545</v>
+      </c>
+      <c r="D41" t="s">
+        <v>219</v>
+      </c>
+      <c r="E41" t="str">
+        <f>B$41&amp;"."&amp;D41</f>
+        <v>NBYTES_MLOFFNO.SMLOE</v>
+      </c>
+      <c r="F41" t="s">
+        <v>220</v>
+      </c>
+      <c r="G41" t="str">
+        <f>"  optional " &amp; IF(C41&gt;0,"uint32", "bool") &amp; " " &amp; D41 &amp; " = "&amp;A41&amp;"; // " &amp; F41</f>
+        <v xml:space="preserve">  optional bool SMLOE = 1; // Source Minor Loop Offset Enable</v>
+      </c>
+      <c r="H41" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" ref="E42:E44" si="7">B$41&amp;"."&amp;D42</f>
+        <v>NBYTES_MLOFFNO.DMLOE</v>
+      </c>
+      <c r="F42" t="s">
+        <v>223</v>
+      </c>
+      <c r="G42" t="str">
+        <f>"  optional " &amp; IF(C42&gt;0,"uint32", "bool") &amp; " " &amp; D42 &amp; " = "&amp;A42&amp;"; // " &amp; F42</f>
+        <v xml:space="preserve">  optional bool DMLOE = 2; // Destination Minor Loop Offset enable</v>
+      </c>
+      <c r="H42" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>30</v>
+      </c>
+      <c r="D43" t="s">
+        <v>216</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="7"/>
+        <v>NBYTES_MLOFFNO.NBYTES</v>
+      </c>
+      <c r="F43" t="s">
+        <v>217</v>
+      </c>
+      <c r="G43" t="str">
+        <f>"  optional " &amp; IF(C43&gt;0,"uint32", "bool") &amp; " " &amp; D43 &amp; " = "&amp;A43&amp;"; // " &amp; F43</f>
+        <v xml:space="preserve">  optional uint32 NBYTES = 3; // Minor Byte Transfer Count</v>
+      </c>
+      <c r="H43" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>546</v>
+      </c>
+      <c r="D44" t="s">
+        <v>219</v>
+      </c>
+      <c r="E44" t="str">
+        <f>B$44&amp;"."&amp;D44</f>
+        <v>NBYTES_MLOFFYES.SMLOE</v>
+      </c>
+      <c r="F44" t="s">
+        <v>220</v>
+      </c>
+      <c r="G44" t="str">
+        <f>"  optional " &amp; IF(C44&gt;0,"uint32", "bool") &amp; " " &amp; D44 &amp; " = "&amp;A44&amp;"; // " &amp; F44</f>
+        <v xml:space="preserve">  optional bool SMLOE = 1; // Source Minor Loop Offset Enable</v>
+      </c>
+      <c r="H44" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>222</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" ref="E45:E47" si="8">B$44&amp;"."&amp;D45</f>
+        <v>NBYTES_MLOFFYES.DMLOE</v>
+      </c>
+      <c r="F45" t="s">
+        <v>223</v>
+      </c>
+      <c r="G45" t="str">
+        <f>"  optional " &amp; IF(C45&gt;0,"uint32", "bool") &amp; " " &amp; D45 &amp; " = "&amp;A45&amp;"; // " &amp; F45</f>
+        <v xml:space="preserve">  optional bool DMLOE = 2; // Destination Minor Loop Offset enable</v>
+      </c>
+      <c r="H45" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+      <c r="D46" t="s">
+        <v>226</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="8"/>
+        <v>NBYTES_MLOFFYES.MLOFF</v>
+      </c>
+      <c r="F46" t="s">
+        <v>228</v>
+      </c>
+      <c r="G46" t="str">
+        <f>"  optional " &amp; IF(C46&gt;0,"uint32", "bool") &amp; " " &amp; D46 &amp; " = "&amp;A46&amp;"; // " &amp; F46</f>
+        <v xml:space="preserve">  optional uint32 MLOFF = 3; // Minor Loop Offset</v>
+      </c>
+      <c r="H46" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
+        <v>216</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="8"/>
+        <v>NBYTES_MLOFFYES.NBYTES</v>
+      </c>
+      <c r="F47" t="s">
+        <v>217</v>
+      </c>
+      <c r="G47" t="str">
+        <f>"  optional " &amp; IF(C47&gt;0,"uint32", "bool") &amp; " " &amp; D47 &amp; " = "&amp;A47&amp;"; // " &amp; F47</f>
+        <v xml:space="preserve">  optional uint32 NBYTES = 4; // Minor Byte Transfer Count</v>
+      </c>
+      <c r="H47" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>229</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" ref="E48:E50" si="9">D48</f>
+        <v>SLAST</v>
+      </c>
+      <c r="F48" t="s">
+        <v>230</v>
+      </c>
+      <c r="H48" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>32</v>
+      </c>
+      <c r="D49" t="s">
+        <v>231</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="9"/>
+        <v>DADDR</v>
+      </c>
+      <c r="F49" t="s">
+        <v>232</v>
+      </c>
+      <c r="H49" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>16</v>
+      </c>
+      <c r="D50" t="s">
+        <v>235</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="9"/>
+        <v>DOFF</v>
+      </c>
+      <c r="F50" t="s">
+        <v>236</v>
+      </c>
+      <c r="H50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>547</v>
+      </c>
+      <c r="D51" t="s">
+        <v>238</v>
+      </c>
+      <c r="E51" t="str">
+        <f>B$51&amp;"."&amp;D51</f>
+        <v>CITER_ELINKYES.ELINK</v>
+      </c>
+      <c r="F51" t="s">
+        <v>239</v>
+      </c>
+      <c r="G51" t="str">
+        <f>"  optional " &amp; IF(C51&gt;0,"uint32", "bool") &amp; " " &amp; D51 &amp; " = "&amp;A51&amp;"; // " &amp; F51</f>
+        <v xml:space="preserve">  optional bool ELINK = 1; // Enable channel-to-channel linking on minor-loop complete</v>
+      </c>
+      <c r="H51" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>241</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" ref="E52:E53" si="10">B$51&amp;"."&amp;D52</f>
+        <v>CITER_ELINKYES.LINKCH</v>
+      </c>
+      <c r="F52" t="s">
+        <v>242</v>
+      </c>
+      <c r="G52" t="str">
+        <f>"  optional " &amp; IF(C52&gt;0,"uint32", "bool") &amp; " " &amp; D52 &amp; " = "&amp;A52&amp;"; // " &amp; F52</f>
+        <v xml:space="preserve">  optional uint32 LINKCH = 2; // Link Channel Number</v>
+      </c>
+      <c r="H52" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>552</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="10"/>
+        <v>CITER_ELINKYES.ITER</v>
+      </c>
+      <c r="F53" t="s">
+        <v>244</v>
+      </c>
+      <c r="G53" t="str">
+        <f>"  optional " &amp; IF(C53&gt;0,"uint32", "bool") &amp; " " &amp; D53 &amp; " = "&amp;A53&amp;"; // " &amp; F53</f>
+        <v xml:space="preserve">  optional uint32 ITER = 3; // Current Major Iteration Count</v>
+      </c>
+      <c r="H53" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>548</v>
+      </c>
+      <c r="D54" t="s">
+        <v>238</v>
+      </c>
+      <c r="E54" t="str">
+        <f>B$54&amp;"."&amp;D54</f>
+        <v>CITER_ELINKNO.ELINK</v>
+      </c>
+      <c r="F54" t="s">
+        <v>239</v>
+      </c>
+      <c r="G54" t="str">
+        <f>"  optional " &amp; IF(C54&gt;0,"uint32", "bool") &amp; " " &amp; D54 &amp; " = "&amp;A54&amp;"; // " &amp; F54</f>
+        <v xml:space="preserve">  optional bool ELINK = 1; // Enable channel-to-channel linking on minor-loop complete</v>
+      </c>
+      <c r="H54" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>552</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" ref="E55:E56" si="11">B$54&amp;"."&amp;D55</f>
+        <v>CITER_ELINKNO.ITER</v>
+      </c>
+      <c r="F55" t="s">
+        <v>244</v>
+      </c>
+      <c r="G55" t="str">
+        <f>"  optional " &amp; IF(C55&gt;0,"uint32", "bool") &amp; " " &amp; D55 &amp; " = "&amp;A55&amp;"; // " &amp; F55</f>
+        <v xml:space="preserve">  optional uint32 ITER = 2; // Current Major Iteration Count</v>
+      </c>
+      <c r="H55" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>32</v>
+      </c>
+      <c r="D56" t="s">
+        <v>247</v>
+      </c>
+      <c r="E56" t="str">
+        <f>D56</f>
+        <v>DLASTSGA</v>
+      </c>
+      <c r="F56" t="s">
+        <v>248</v>
+      </c>
+      <c r="H56" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>549</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>250</v>
+      </c>
+      <c r="E57" t="str">
+        <f>B$57&amp;"."&amp;D57</f>
+        <v>CSR.BWC</v>
+      </c>
+      <c r="F57" t="s">
+        <v>251</v>
+      </c>
+      <c r="G57" t="str">
+        <f>"  optional " &amp; IF(C57&gt;0,"uint32", "bool") &amp; " " &amp; D57 &amp; " = "&amp;A57&amp;"; // " &amp; F57</f>
+        <v xml:space="preserve">  optional uint32 BWC = 1; // Bandwidth Control</v>
+      </c>
+      <c r="H57" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>253</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" ref="E58:E66" si="12">B$57&amp;"."&amp;D58</f>
+        <v>CSR.MAJORLINKCH</v>
+      </c>
+      <c r="F58" t="s">
+        <v>242</v>
+      </c>
+      <c r="G58" t="str">
+        <f>"  optional " &amp; IF(C58&gt;0,"uint32", "bool") &amp; " " &amp; D58 &amp; " = "&amp;A58&amp;"; // " &amp; F58</f>
+        <v xml:space="preserve">  optional uint32 MAJORLINKCH = 2; // Link Channel Number</v>
+      </c>
+      <c r="H58" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>255</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="12"/>
+        <v>CSR.DONE</v>
+      </c>
+      <c r="F59" t="s">
+        <v>256</v>
+      </c>
+      <c r="G59" t="str">
+        <f>"  optional " &amp; IF(C59&gt;0,"uint32", "bool") &amp; " " &amp; D59 &amp; " = "&amp;A59&amp;"; // " &amp; F59</f>
+        <v xml:space="preserve">  optional bool DONE = 3; // Channel Done</v>
+      </c>
+      <c r="H59" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>258</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="12"/>
+        <v>CSR.ACTIVE</v>
+      </c>
+      <c r="F60" t="s">
+        <v>259</v>
+      </c>
+      <c r="G60" t="str">
+        <f>"  optional " &amp; IF(C60&gt;0,"uint32", "bool") &amp; " " &amp; D60 &amp; " = "&amp;A60&amp;"; // " &amp; F60</f>
+        <v xml:space="preserve">  optional bool ACTIVE = 4; // Channel Active</v>
+      </c>
+      <c r="H60" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>261</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="12"/>
+        <v>CSR.MAJORELINK</v>
+      </c>
+      <c r="F61" t="s">
+        <v>262</v>
+      </c>
+      <c r="G61" t="str">
+        <f>"  optional " &amp; IF(C61&gt;0,"uint32", "bool") &amp; " " &amp; D61 &amp; " = "&amp;A61&amp;"; // " &amp; F61</f>
+        <v xml:space="preserve">  optional bool MAJORELINK = 5; // Enable channel-to-channel linking on major loop complete</v>
+      </c>
+      <c r="H61" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>264</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="12"/>
+        <v>CSR.ESG</v>
+      </c>
+      <c r="F62" t="s">
+        <v>265</v>
+      </c>
+      <c r="G62" t="str">
+        <f>"  optional " &amp; IF(C62&gt;0,"uint32", "bool") &amp; " " &amp; D62 &amp; " = "&amp;A62&amp;"; // " &amp; F62</f>
+        <v xml:space="preserve">  optional bool ESG = 6; // Enable Scatter/Gather Processing</v>
+      </c>
+      <c r="H62" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>267</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="12"/>
+        <v>CSR.DREQ</v>
+      </c>
+      <c r="F63" t="s">
+        <v>268</v>
+      </c>
+      <c r="G63" t="str">
+        <f>"  optional " &amp; IF(C63&gt;0,"uint32", "bool") &amp; " " &amp; D63 &amp; " = "&amp;A63&amp;"; // " &amp; F63</f>
+        <v xml:space="preserve">  optional bool DREQ = 7; // Disable Request</v>
+      </c>
+      <c r="H63" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>270</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="12"/>
+        <v>CSR.INTHALF</v>
+      </c>
+      <c r="F64" t="s">
+        <v>271</v>
+      </c>
+      <c r="G64" t="str">
+        <f>"  optional " &amp; IF(C64&gt;0,"uint32", "bool") &amp; " " &amp; D64 &amp; " = "&amp;A64&amp;"; // " &amp; F64</f>
+        <v xml:space="preserve">  optional bool INTHALF = 8; // Enable an interrupt when major counter is half complete.</v>
+      </c>
+      <c r="H64" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>273</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="12"/>
+        <v>CSR.INTMAJOR</v>
+      </c>
+      <c r="F65" t="s">
+        <v>274</v>
+      </c>
+      <c r="G65" t="str">
+        <f>"  optional " &amp; IF(C65&gt;0,"uint32", "bool") &amp; " " &amp; D65 &amp; " = "&amp;A65&amp;"; // " &amp; F65</f>
+        <v xml:space="preserve">  optional bool INTMAJOR = 9; // Enable an interrupt when major iteration count completes</v>
+      </c>
+      <c r="H65" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>276</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="12"/>
+        <v>CSR.START</v>
+      </c>
+      <c r="F66" t="s">
+        <v>277</v>
+      </c>
+      <c r="G66" t="str">
+        <f>"  optional " &amp; IF(C66&gt;0,"uint32", "bool") &amp; " " &amp; D66 &amp; " = "&amp;A66&amp;"; // " &amp; F66</f>
+        <v xml:space="preserve">  optional bool START = 10; // Channel Start</v>
+      </c>
+      <c r="H66" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>550</v>
+      </c>
+      <c r="D67" t="s">
+        <v>238</v>
+      </c>
+      <c r="E67" t="str">
+        <f>B$67&amp;"."&amp;D67</f>
+        <v>BITER_ELINKYES.ELINK</v>
+      </c>
+      <c r="F67" t="s">
+        <v>239</v>
+      </c>
+      <c r="G67" t="str">
+        <f>"  optional " &amp; IF(C67&gt;0,"uint32", "bool") &amp; " " &amp; D67 &amp; " = "&amp;A67&amp;"; // " &amp; F67</f>
+        <v xml:space="preserve">  optional bool ELINK = 1; // Enable channel-to-channel linking on minor-loop complete</v>
+      </c>
+      <c r="H67" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>241</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" ref="E68:E69" si="13">B$67&amp;"."&amp;D68</f>
+        <v>BITER_ELINKYES.LINKCH</v>
+      </c>
+      <c r="F68" t="s">
+        <v>242</v>
+      </c>
+      <c r="G68" t="str">
+        <f>"  optional " &amp; IF(C68&gt;0,"uint32", "bool") &amp; " " &amp; D68 &amp; " = "&amp;A68&amp;"; // " &amp; F68</f>
+        <v xml:space="preserve">  optional uint32 LINKCH = 2; // Link Channel Number</v>
+      </c>
+      <c r="H68" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <v>9</v>
+      </c>
+      <c r="D69" t="s">
+        <v>552</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="13"/>
+        <v>BITER_ELINKYES.ITER</v>
+      </c>
+      <c r="F69" t="s">
+        <v>244</v>
+      </c>
+      <c r="G69" t="str">
+        <f>"  optional " &amp; IF(C69&gt;0,"uint32", "bool") &amp; " " &amp; D69 &amp; " = "&amp;A69&amp;"; // " &amp; F69</f>
+        <v xml:space="preserve">  optional uint32 ITER = 3; // Current Major Iteration Count</v>
+      </c>
+      <c r="H69" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>551</v>
+      </c>
+      <c r="D70" t="s">
+        <v>238</v>
+      </c>
+      <c r="E70" t="str">
+        <f>B$70&amp;"."&amp;D70</f>
+        <v>BITER_ELINKNO.ELINK</v>
+      </c>
+      <c r="F70" t="s">
+        <v>239</v>
+      </c>
+      <c r="G70" t="str">
+        <f>"  optional " &amp; IF(C70&gt;0,"uint32", "bool") &amp; " " &amp; D70 &amp; " = "&amp;A70&amp;"; // " &amp; F70</f>
+        <v xml:space="preserve">  optional bool ELINK = 1; // Enable channel-to-channel linking on minor-loop complete</v>
+      </c>
+      <c r="H70" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="C71">
+        <v>15</v>
+      </c>
+      <c r="D71" t="s">
+        <v>552</v>
+      </c>
+      <c r="E71" t="str">
+        <f>B$70&amp;"."&amp;D71</f>
+        <v>BITER_ELINKNO.ITER</v>
+      </c>
+      <c r="F71" t="s">
+        <v>244</v>
+      </c>
+      <c r="G71" t="str">
+        <f>"  optional " &amp; IF(C71&gt;0,"uint32", "bool") &amp; " " &amp; D71 &amp; " = "&amp;A71&amp;"; // " &amp; F71</f>
+        <v xml:space="preserve">  optional uint32 ITER = 2; // Current Major Iteration Count</v>
+      </c>
+      <c r="H71" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M41"/>
   <sheetViews>
@@ -4043,13 +4451,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="C1" t="s">
-        <v>357</v>
+        <v>340</v>
       </c>
       <c r="D1" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="E1">
         <v>32</v>
@@ -4061,7 +4469,7 @@
         <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="J1" t="str">
         <f>"  optional uint"&amp;E1&amp;" "&amp;D1&amp;" = "&amp;A1&amp;";  // "&amp;C1&amp;" ("&amp;H1&amp;")"</f>
@@ -4073,13 +4481,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="C2" t="s">
-        <v>358</v>
+        <v>341</v>
       </c>
       <c r="D2" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="E2">
         <v>32</v>
@@ -4091,7 +4499,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:J22" si="0">"  optional uint"&amp;E2&amp;" "&amp;D2&amp;" = "&amp;A2&amp;";  // "&amp;C2&amp;" ("&amp;H2&amp;")"</f>
@@ -4103,13 +4511,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
       <c r="D3" t="s">
-        <v>382</v>
+        <v>365</v>
       </c>
       <c r="E3">
         <v>32</v>
@@ -4118,10 +4526,10 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="H3" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
@@ -4133,13 +4541,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="C4" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
       <c r="D4" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="E4">
         <v>32</v>
@@ -4151,7 +4559,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
@@ -4163,13 +4571,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="C5" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="D5" t="s">
-        <v>384</v>
+        <v>367</v>
       </c>
       <c r="E5">
         <v>32</v>
@@ -4181,7 +4589,7 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
@@ -4193,13 +4601,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
       <c r="D6" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="E6">
         <v>32</v>
@@ -4211,7 +4619,7 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
@@ -4223,13 +4631,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="C7" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="D7" t="s">
-        <v>386</v>
+        <v>369</v>
       </c>
       <c r="E7">
         <v>32</v>
@@ -4241,7 +4649,7 @@
         <v>86</v>
       </c>
       <c r="H7" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
@@ -4253,13 +4661,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="C8" t="s">
-        <v>364</v>
+        <v>347</v>
       </c>
       <c r="D8" t="s">
-        <v>387</v>
+        <v>370</v>
       </c>
       <c r="E8">
         <v>32</v>
@@ -4271,7 +4679,7 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
@@ -4283,13 +4691,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="C9" t="s">
-        <v>365</v>
+        <v>348</v>
       </c>
       <c r="D9" t="s">
-        <v>388</v>
+        <v>371</v>
       </c>
       <c r="E9">
         <v>32</v>
@@ -4301,7 +4709,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
@@ -4313,13 +4721,13 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="C10" t="s">
-        <v>366</v>
+        <v>349</v>
       </c>
       <c r="D10" t="s">
-        <v>389</v>
+        <v>372</v>
       </c>
       <c r="E10">
         <v>32</v>
@@ -4331,7 +4739,7 @@
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
@@ -4343,13 +4751,13 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="C11" t="s">
-        <v>367</v>
+        <v>350</v>
       </c>
       <c r="D11" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="E11">
         <v>32</v>
@@ -4358,10 +4766,10 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="H11" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
@@ -4373,13 +4781,13 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="C12" t="s">
-        <v>368</v>
+        <v>351</v>
       </c>
       <c r="D12" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="E12">
         <v>32</v>
@@ -4388,10 +4796,10 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="H12" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
@@ -4403,13 +4811,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="C13" t="s">
-        <v>369</v>
+        <v>352</v>
       </c>
       <c r="D13" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="E13">
         <v>32</v>
@@ -4418,10 +4826,10 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
       <c r="H13" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
@@ -4433,13 +4841,13 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="C14" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
       <c r="D14" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="E14">
         <v>32</v>
@@ -4448,10 +4856,10 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="H14" t="s">
-        <v>340</v>
+        <v>323</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
@@ -4463,13 +4871,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="C15" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="D15" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="E15">
         <v>32</v>
@@ -4481,7 +4889,7 @@
         <v>52</v>
       </c>
       <c r="H15" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
@@ -4493,13 +4901,13 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="C16" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="D16" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="E16">
         <v>32</v>
@@ -4511,7 +4919,7 @@
         <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
@@ -4523,13 +4931,13 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="C17" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="D17" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="E17">
         <v>32</v>
@@ -4541,7 +4949,7 @@
         <v>52</v>
       </c>
       <c r="H17" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
@@ -4553,13 +4961,13 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="C18" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="D18" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="E18">
         <v>32</v>
@@ -4571,7 +4979,7 @@
         <v>52</v>
       </c>
       <c r="H18" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
@@ -4583,13 +4991,13 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="C19" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
       <c r="D19" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="E19">
         <v>32</v>
@@ -4601,7 +5009,7 @@
         <v>52</v>
       </c>
       <c r="H19" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
@@ -4613,13 +5021,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="C20" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="D20" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
       <c r="E20">
         <v>32</v>
@@ -4631,7 +5039,7 @@
         <v>52</v>
       </c>
       <c r="H20" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
@@ -4643,13 +5051,13 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="C21" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="D21" t="s">
-        <v>400</v>
+        <v>383</v>
       </c>
       <c r="E21">
         <v>32</v>
@@ -4661,7 +5069,7 @@
         <v>52</v>
       </c>
       <c r="H21" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
@@ -4673,13 +5081,13 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="C22" t="s">
-        <v>379</v>
+        <v>362</v>
       </c>
       <c r="D22" t="s">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="E22">
         <v>32</v>
@@ -4691,7 +5099,7 @@
         <v>52</v>
       </c>
       <c r="H22" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
@@ -4700,7 +5108,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>370</v>
+        <v>353</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -4711,10 +5119,10 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="D25" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="F25" t="str">
         <f>"    result.has_"&amp;D25&amp;" = true;  // "&amp;C25&amp;"
@@ -4723,11 +5131,11 @@
     result.ADC0 = SIM_SCGC6 &amp; SIM_SCGC6_ADC0;</v>
       </c>
       <c r="J25" t="str">
-        <f>"  optional bool "&amp;D25&amp;" = "&amp;A25&amp;";  // "&amp;C25</f>
+        <f t="shared" ref="J25:J38" si="1">"  optional bool "&amp;D25&amp;" = "&amp;A25&amp;";  // "&amp;C25</f>
         <v xml:space="preserve">  optional bool RTC = 1;  // RTC Access Control</v>
       </c>
       <c r="M25" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -4738,23 +5146,23 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="D26" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" ref="F26:F38" si="1">"    result.has_"&amp;D26&amp;" = true;  // "&amp;C26&amp;"
+        <f t="shared" ref="F26:F38" si="2">"    result.has_"&amp;D26&amp;" = true;  // "&amp;C26&amp;"
     result."&amp;D27&amp;" = "&amp;A$24&amp;" &amp; "&amp;A$24&amp;"_"&amp;D27&amp;";"</f>
         <v xml:space="preserve">    result.has_ADC0 = true;  // ADC0 Clock Gate Control
     result.FTM1 = SIM_SCGC6 &amp; SIM_SCGC6_FTM1;</v>
       </c>
       <c r="J26" t="str">
-        <f>"  optional bool "&amp;D26&amp;" = "&amp;A26&amp;";  // "&amp;C26</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool ADC0 = 2;  // ADC0 Clock Gate Control</v>
       </c>
       <c r="M26" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -4765,22 +5173,22 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="D27" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_FTM1 = true;  // FTM1 Clock Gate Control
     result.FTM0 = SIM_SCGC6 &amp; SIM_SCGC6_FTM0;</v>
       </c>
       <c r="J27" t="str">
-        <f>"  optional bool "&amp;D27&amp;" = "&amp;A27&amp;";  // "&amp;C27</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool FTM1 = 3;  // FTM1 Clock Gate Control</v>
       </c>
       <c r="M27" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -4791,22 +5199,22 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="D28" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_FTM0 = true;  // FTM0 Clock Gate Control
     result.PIT = SIM_SCGC6 &amp; SIM_SCGC6_PIT;</v>
       </c>
       <c r="J28" t="str">
-        <f>"  optional bool "&amp;D28&amp;" = "&amp;A28&amp;";  // "&amp;C28</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool FTM0 = 4;  // FTM0 Clock Gate Control</v>
       </c>
       <c r="M28" t="s">
-        <v>413</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -4817,22 +5225,22 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="D29" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_PIT = true;  // PIT Clock Gate Control
     result.PDB = SIM_SCGC6 &amp; SIM_SCGC6_PDB;</v>
       </c>
       <c r="J29" t="str">
-        <f>"  optional bool "&amp;D29&amp;" = "&amp;A29&amp;";  // "&amp;C29</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool PIT = 5;  // PIT Clock Gate Control</v>
       </c>
       <c r="M29" t="s">
-        <v>416</v>
+        <v>399</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -4843,22 +5251,22 @@
         <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="D30" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_PDB = true;  // PDB Clock Gate Control
     result.USBDCD = SIM_SCGC6 &amp; SIM_SCGC6_USBDCD;</v>
       </c>
       <c r="J30" t="str">
-        <f>"  optional bool "&amp;D30&amp;" = "&amp;A30&amp;";  // "&amp;C30</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool PDB = 6;  // PDB Clock Gate Control</v>
       </c>
       <c r="M30" t="s">
-        <v>419</v>
+        <v>402</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -4869,22 +5277,22 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="D31" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_USBDCD = true;  // USB DCD Clock Gate Control
     result.CRC = SIM_SCGC6 &amp; SIM_SCGC6_CRC;</v>
       </c>
       <c r="J31" t="str">
-        <f>"  optional bool "&amp;D31&amp;" = "&amp;A31&amp;";  // "&amp;C31</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool USBDCD = 7;  // USB DCD Clock Gate Control</v>
       </c>
       <c r="M31" t="s">
-        <v>422</v>
+        <v>405</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -4895,22 +5303,22 @@
         <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D32" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_CRC = true;  // CRC Clock Gate Control
     result.I2S = SIM_SCGC6 &amp; SIM_SCGC6_I2S;</v>
       </c>
       <c r="J32" t="str">
-        <f>"  optional bool "&amp;D32&amp;" = "&amp;A32&amp;";  // "&amp;C32</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool CRC = 8;  // CRC Clock Gate Control</v>
       </c>
       <c r="M32" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -4921,22 +5329,22 @@
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="D33" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_I2S = true;  // I2S Clock Gate Control
     result.SPI1 = SIM_SCGC6 &amp; SIM_SCGC6_SPI1;</v>
       </c>
       <c r="J33" t="str">
-        <f>"  optional bool "&amp;D33&amp;" = "&amp;A33&amp;";  // "&amp;C33</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool I2S = 9;  // I2S Clock Gate Control</v>
       </c>
       <c r="M33" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -4947,22 +5355,22 @@
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="D34" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_SPI1 = true;  // SPI1 Clock Gate Control
     result.SPI0 = SIM_SCGC6 &amp; SIM_SCGC6_SPI0;</v>
       </c>
       <c r="J34" t="str">
-        <f>"  optional bool "&amp;D34&amp;" = "&amp;A34&amp;";  // "&amp;C34</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool SPI1 = 10;  // SPI1 Clock Gate Control</v>
       </c>
       <c r="M34" t="s">
-        <v>431</v>
+        <v>414</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -4973,22 +5381,22 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="D35" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_SPI0 = true;  // SPI0 Clock Gate Control
     result.FLEXCAN0 = SIM_SCGC6 &amp; SIM_SCGC6_FLEXCAN0;</v>
       </c>
       <c r="J35" t="str">
-        <f>"  optional bool "&amp;D35&amp;" = "&amp;A35&amp;";  // "&amp;C35</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool SPI0 = 11;  // SPI0 Clock Gate Control</v>
       </c>
       <c r="M35" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -4999,22 +5407,22 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
       <c r="D36" t="s">
-        <v>435</v>
+        <v>418</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_FLEXCAN0 = true;  // FlexCAN0 Clock Gate Control
     result.DMAMUX = SIM_SCGC6 &amp; SIM_SCGC6_DMAMUX;</v>
       </c>
       <c r="J36" t="str">
-        <f>"  optional bool "&amp;D36&amp;" = "&amp;A36&amp;";  // "&amp;C36</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool FLEXCAN0 = 12;  // FlexCAN0 Clock Gate Control</v>
       </c>
       <c r="M36" t="s">
-        <v>437</v>
+        <v>420</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -5025,22 +5433,22 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
       <c r="D37" t="s">
-        <v>438</v>
+        <v>421</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_DMAMUX = true;  // DMA Mux Clock Gate Control
     result.FTFL = SIM_SCGC6 &amp; SIM_SCGC6_FTFL;</v>
       </c>
       <c r="J37" t="str">
-        <f>"  optional bool "&amp;D37&amp;" = "&amp;A37&amp;";  // "&amp;C37</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool DMAMUX = 13;  // DMA Mux Clock Gate Control</v>
       </c>
       <c r="M37" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -5051,27 +5459,27 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="D38" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">    result.has_FTFL = true;  // Flash Memory Clock Gate Control
     result. = SIM_SCGC6 &amp; SIM_SCGC6_;</v>
       </c>
       <c r="J38" t="str">
-        <f>"  optional bool "&amp;D38&amp;" = "&amp;A38&amp;";  // "&amp;C38</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  optional bool FTFL = 14;  // Flash Memory Clock Gate Control</v>
       </c>
       <c r="M38" t="s">
-        <v>443</v>
+        <v>426</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
@@ -5082,17 +5490,17 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
       <c r="D41" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="J41" t="str">
         <f>"  optional bool "&amp;D41&amp;" = "&amp;A41&amp;";  // "&amp;C41</f>
         <v xml:space="preserve">  optional bool DMA = 1;  // DMA Clock Gate Control</v>
       </c>
       <c r="M41" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -5101,576 +5509,579 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
       <c r="C1" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="D1" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>450</v>
+        <v>433</v>
       </c>
       <c r="C2" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
       <c r="C3" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>454</v>
+        <v>437</v>
       </c>
       <c r="C4" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>455</v>
+        <v>438</v>
       </c>
       <c r="C5" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
       <c r="C6" t="s">
-        <v>457</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>458</v>
+        <v>441</v>
       </c>
       <c r="C7" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
       <c r="C8" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="C9" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
       <c r="C10" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="C11" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="C12" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="C13" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="C14" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
       <c r="C15" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>471</v>
+        <v>454</v>
       </c>
       <c r="C16" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
       <c r="C17" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
       <c r="C18" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>474</v>
+        <v>457</v>
       </c>
       <c r="C19" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="C20" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="C21" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>477</v>
+        <v>460</v>
       </c>
       <c r="C22" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="B23" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="C23" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="D23" t="s">
-        <v>481</v>
+        <v>464</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="B24" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c r="C24" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
       <c r="D24" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="B25" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
       <c r="C25" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="B26" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="C26" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="B27" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
       <c r="C27" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="D27" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="B28" t="s">
-        <v>493</v>
+        <v>476</v>
       </c>
       <c r="C28" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
       <c r="D28" t="s">
-        <v>495</v>
+        <v>478</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="B29" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
       <c r="C29" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
       <c r="D29" t="s">
-        <v>498</v>
+        <v>481</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="B30" t="s">
-        <v>499</v>
+        <v>482</v>
       </c>
       <c r="C30" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
       <c r="D30" t="s">
-        <v>501</v>
+        <v>484</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="B31" t="s">
-        <v>502</v>
+        <v>485</v>
       </c>
       <c r="C31" t="s">
-        <v>503</v>
+        <v>486</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
       <c r="B32" t="s">
-        <v>505</v>
+        <v>488</v>
       </c>
       <c r="C32" t="s">
-        <v>506</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
       <c r="B33" t="s">
-        <v>507</v>
+        <v>490</v>
       </c>
       <c r="C33" t="s">
-        <v>508</v>
+        <v>491</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
       <c r="B34" t="s">
-        <v>509</v>
+        <v>492</v>
       </c>
       <c r="C34" t="s">
-        <v>510</v>
+        <v>493</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
       <c r="B35" t="s">
-        <v>511</v>
+        <v>494</v>
       </c>
       <c r="C35" t="s">
-        <v>512</v>
+        <v>495</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="B36" t="s">
-        <v>514</v>
+        <v>497</v>
       </c>
       <c r="C36" t="s">
-        <v>506</v>
+        <v>489</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="B37" t="s">
-        <v>515</v>
+        <v>498</v>
       </c>
       <c r="C37" t="s">
-        <v>508</v>
+        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="B38" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
       <c r="C38" t="s">
-        <v>510</v>
+        <v>493</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="B39" t="s">
-        <v>517</v>
+        <v>500</v>
       </c>
       <c r="C39" t="s">
-        <v>512</v>
+        <v>495</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
       <c r="B40" t="s">
-        <v>519</v>
+        <v>502</v>
       </c>
       <c r="C40" t="s">
-        <v>520</v>
+        <v>503</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
       <c r="B41" t="s">
-        <v>521</v>
+        <v>504</v>
       </c>
       <c r="C41" t="s">
-        <v>522</v>
+        <v>505</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
       <c r="B42" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
       <c r="C42" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
       <c r="D42" t="s">
-        <v>525</v>
+        <v>508</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
       <c r="B43" t="s">
-        <v>527</v>
+        <v>510</v>
       </c>
       <c r="C43" t="s">
-        <v>528</v>
+        <v>511</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
       <c r="B44" t="s">
-        <v>529</v>
+        <v>512</v>
       </c>
       <c r="C44" t="s">
-        <v>530</v>
+        <v>513</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
       <c r="B45" t="s">
-        <v>531</v>
+        <v>514</v>
       </c>
       <c r="C45" t="s">
-        <v>532</v>
+        <v>515</v>
       </c>
       <c r="D45" t="s">
-        <v>533</v>
+        <v>516</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
       <c r="B46" t="s">
-        <v>534</v>
+        <v>517</v>
       </c>
       <c r="C46" t="s">
-        <v>535</v>
+        <v>518</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
       <c r="B47" t="s">
-        <v>536</v>
+        <v>519</v>
       </c>
       <c r="C47" t="s">
-        <v>537</v>
+        <v>520</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
       <c r="B48" t="s">
-        <v>539</v>
+        <v>522</v>
       </c>
       <c r="C48" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
       <c r="D48" t="s">
-        <v>541</v>
+        <v>524</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
       <c r="B49" t="s">
-        <v>542</v>
+        <v>525</v>
       </c>
       <c r="C49" t="s">
-        <v>543</v>
+        <v>526</v>
       </c>
       <c r="D49" t="s">
-        <v>544</v>
+        <v>527</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
       <c r="B50" t="s">
-        <v>545</v>
+        <v>528</v>
       </c>
       <c r="C50" t="s">
-        <v>546</v>
+        <v>529</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
       <c r="B51" t="s">
-        <v>547</v>
+        <v>530</v>
       </c>
       <c r="C51" t="s">
-        <v>548</v>
+        <v>531</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
       <c r="B52" t="s">
-        <v>549</v>
+        <v>532</v>
       </c>
       <c r="C52" t="s">
-        <v>550</v>
+        <v>533</v>
       </c>
       <c r="D52" t="s">
-        <v>551</v>
+        <v>534</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
       <c r="B53" t="s">
-        <v>552</v>
+        <v>535</v>
       </c>
       <c r="C53" t="s">
-        <v>553</v>
+        <v>536</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>521</v>
+      </c>
+      <c r="B54" t="s">
+        <v>537</v>
+      </c>
+      <c r="C54" t="s">
         <v>538</v>
-      </c>
-      <c r="B54" t="s">
-        <v>554</v>
-      </c>
-      <c r="C54" t="s">
-        <v>555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ADC memory map
</commit_message>
<xml_diff>
--- a/teensy_minimal_rpc/notebooks/register-field-descriptions.xlsx
+++ b/teensy_minimal_rpc/notebooks/register-field-descriptions.xlsx
@@ -13,11 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="dma mem map" sheetId="1" r:id="rId1"/>
-    <sheet name="dma registers" sheetId="4" r:id="rId2"/>
-    <sheet name="sim" sheetId="2" r:id="rId3"/>
-    <sheet name="adc" sheetId="3" r:id="rId4"/>
+    <sheet name="dma registers" sheetId="2" r:id="rId2"/>
+    <sheet name="sim" sheetId="3" r:id="rId3"/>
+    <sheet name="adc" sheetId="4" r:id="rId4"/>
+    <sheet name="adc mem map" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Christian Fobel - Personal View" guid="{FB44FD47-0B92-4391-9CB5-FFD8B50F36C3}" mergeInterval="0" personalView="1" xWindow="1200" windowWidth="1200" windowHeight="1450" activeSheetId="2"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="650">
   <si>
     <t>4000_8000</t>
   </si>
@@ -1686,6 +1690,297 @@
   </si>
   <si>
     <t>ITER</t>
+  </si>
+  <si>
+    <t>4003_B000</t>
+  </si>
+  <si>
+    <t>ADC Status and Control Registers 1</t>
+  </si>
+  <si>
+    <t>0000_001Fh</t>
+  </si>
+  <si>
+    <t>31.3.1/653</t>
+  </si>
+  <si>
+    <t>4003_B004</t>
+  </si>
+  <si>
+    <t>4003_B008</t>
+  </si>
+  <si>
+    <t>ADC Configuration Register 1</t>
+  </si>
+  <si>
+    <t>31.3.2/656</t>
+  </si>
+  <si>
+    <t>4003_B00C</t>
+  </si>
+  <si>
+    <t>ADC Configuration Register 2</t>
+  </si>
+  <si>
+    <t>31.3.3/658</t>
+  </si>
+  <si>
+    <t>4003_B010</t>
+  </si>
+  <si>
+    <t>31.3.4/659</t>
+  </si>
+  <si>
+    <t>4003_B014</t>
+  </si>
+  <si>
+    <t>4003_B018</t>
+  </si>
+  <si>
+    <t>Compare Value Registers</t>
+  </si>
+  <si>
+    <t>31.3.5/660</t>
+  </si>
+  <si>
+    <t>4003_B01C</t>
+  </si>
+  <si>
+    <t>4003_B020</t>
+  </si>
+  <si>
+    <t>Status and Control Register 2</t>
+  </si>
+  <si>
+    <t>31.3.6/661</t>
+  </si>
+  <si>
+    <t>4003_B024</t>
+  </si>
+  <si>
+    <t>Status and Control Register 3</t>
+  </si>
+  <si>
+    <t>31.3.7/663</t>
+  </si>
+  <si>
+    <t>4003_B028</t>
+  </si>
+  <si>
+    <t>0000_0004h</t>
+  </si>
+  <si>
+    <t>31.3.8/665</t>
+  </si>
+  <si>
+    <t>4003_B02C</t>
+  </si>
+  <si>
+    <t>0000_8200h</t>
+  </si>
+  <si>
+    <t>31.3.9/665</t>
+  </si>
+  <si>
+    <t>4003_B030</t>
+  </si>
+  <si>
+    <t>31.3.10/666</t>
+  </si>
+  <si>
+    <t>4003_B034</t>
+  </si>
+  <si>
+    <t>0000_000Ah</t>
+  </si>
+  <si>
+    <t>31.3.11/666</t>
+  </si>
+  <si>
+    <t>4003_B038</t>
+  </si>
+  <si>
+    <t>0000_0020h</t>
+  </si>
+  <si>
+    <t>31.3.12/667</t>
+  </si>
+  <si>
+    <t>4003_B03C</t>
+  </si>
+  <si>
+    <t>0000_0200h</t>
+  </si>
+  <si>
+    <t>31.3.13/667</t>
+  </si>
+  <si>
+    <t>4003_B040</t>
+  </si>
+  <si>
+    <t>0000_0100h</t>
+  </si>
+  <si>
+    <t>31.3.14/668</t>
+  </si>
+  <si>
+    <t>4003_B044</t>
+  </si>
+  <si>
+    <t>0000_0080h</t>
+  </si>
+  <si>
+    <t>31.3.15/668</t>
+  </si>
+  <si>
+    <t>4003_B048</t>
+  </si>
+  <si>
+    <t>0000_0040h</t>
+  </si>
+  <si>
+    <t>31.3.16/669</t>
+  </si>
+  <si>
+    <t>4003_B04C</t>
+  </si>
+  <si>
+    <t>31.3.17/669</t>
+  </si>
+  <si>
+    <t>4003_B050</t>
+  </si>
+  <si>
+    <t>ADC PGA Register</t>
+  </si>
+  <si>
+    <t>31.3.18/670</t>
+  </si>
+  <si>
+    <t>4003_B054</t>
+  </si>
+  <si>
+    <t>31.3.19/671</t>
+  </si>
+  <si>
+    <t>4003_B058</t>
+  </si>
+  <si>
+    <t>31.3.20/672</t>
+  </si>
+  <si>
+    <t>4003_B05C</t>
+  </si>
+  <si>
+    <t>31.3.21/672</t>
+  </si>
+  <si>
+    <t>4003_B060</t>
+  </si>
+  <si>
+    <t>31.3.22/673</t>
+  </si>
+  <si>
+    <t>4003_B064</t>
+  </si>
+  <si>
+    <t>31.3.23/673</t>
+  </si>
+  <si>
+    <t>4003_B068</t>
+  </si>
+  <si>
+    <t>31.3.24/674</t>
+  </si>
+  <si>
+    <t>4003_B06C</t>
+  </si>
+  <si>
+    <t>31.3.25/674</t>
+  </si>
+  <si>
+    <t>400B_B000</t>
+  </si>
+  <si>
+    <t>400B_B004</t>
+  </si>
+  <si>
+    <t>400B_B008</t>
+  </si>
+  <si>
+    <t>400B_B00C</t>
+  </si>
+  <si>
+    <t>400B_B010</t>
+  </si>
+  <si>
+    <t>400B_B014</t>
+  </si>
+  <si>
+    <t>400B_B018</t>
+  </si>
+  <si>
+    <t>400B_B01C</t>
+  </si>
+  <si>
+    <t>400B_B020</t>
+  </si>
+  <si>
+    <t>400B_B024</t>
+  </si>
+  <si>
+    <t>400B_B028</t>
+  </si>
+  <si>
+    <t>400B_B02C</t>
+  </si>
+  <si>
+    <t>400B_B030</t>
+  </si>
+  <si>
+    <t>400B_B034</t>
+  </si>
+  <si>
+    <t>400B_B038</t>
+  </si>
+  <si>
+    <t>400B_B03C</t>
+  </si>
+  <si>
+    <t>400B_B040</t>
+  </si>
+  <si>
+    <t>400B_B044</t>
+  </si>
+  <si>
+    <t>400B_B048</t>
+  </si>
+  <si>
+    <t>400B_B04C</t>
+  </si>
+  <si>
+    <t>400B_B050</t>
+  </si>
+  <si>
+    <t>400B_B054</t>
+  </si>
+  <si>
+    <t>400B_B058</t>
+  </si>
+  <si>
+    <t>400B_B05C</t>
+  </si>
+  <si>
+    <t>400B_B060</t>
+  </si>
+  <si>
+    <t>400B_B064</t>
+  </si>
+  <si>
+    <t>400B_B068</t>
+  </si>
+  <si>
+    <t>400B_B06C</t>
   </si>
 </sst>
 </file>
@@ -1738,6 +2033,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FD2A050E-2A98-406D-AD5E-BA26E8C945F5}">
+  <header guid="{FD2A050E-2A98-406D-AD5E-BA26E8C945F5}" dateTime="2015-11-03T14:16:09" maxSheetId="6" userName="Christian Fobel" r:id="rId1">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2005,15 +2322,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:G116"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="94.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
@@ -2921,6 +3238,12 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{FB44FD47-0B92-4391-9CB5-FFD8B50F36C3}" scale="80">
+      <selection activeCell="A45" sqref="A45"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2929,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4425,6 +4748,12 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{FB44FD47-0B92-4391-9CB5-FFD8B50F36C3}" scale="85" topLeftCell="B1">
+      <selection activeCell="C46" sqref="C46"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5504,8 +5833,14 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{FB44FD47-0B92-4391-9CB5-FFD8B50F36C3}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5513,7 +5848,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6085,6 +6422,1330 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{FB44FD47-0B92-4391-9CB5-FFD8B50F36C3}">
+      <selection activeCell="A23" sqref="A23"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D1">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>555</v>
+      </c>
+      <c r="G1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B2" t="s">
+        <v>554</v>
+      </c>
+      <c r="C2" t="s">
+        <v>496</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>555</v>
+      </c>
+      <c r="G2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>558</v>
+      </c>
+      <c r="B3" t="s">
+        <v>559</v>
+      </c>
+      <c r="C3" t="s">
+        <v>472</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B4" t="s">
+        <v>562</v>
+      </c>
+      <c r="C4" t="s">
+        <v>461</v>
+      </c>
+      <c r="D4">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>564</v>
+      </c>
+      <c r="B5" t="s">
+        <v>442</v>
+      </c>
+      <c r="C5" t="s">
+        <v>443</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>566</v>
+      </c>
+      <c r="B6" t="s">
+        <v>442</v>
+      </c>
+      <c r="C6" t="s">
+        <v>441</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>567</v>
+      </c>
+      <c r="B7" t="s">
+        <v>568</v>
+      </c>
+      <c r="C7" t="s">
+        <v>455</v>
+      </c>
+      <c r="D7">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>570</v>
+      </c>
+      <c r="B8" t="s">
+        <v>568</v>
+      </c>
+      <c r="C8" t="s">
+        <v>452</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>571</v>
+      </c>
+      <c r="B9" t="s">
+        <v>572</v>
+      </c>
+      <c r="C9" t="s">
+        <v>521</v>
+      </c>
+      <c r="D9">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>574</v>
+      </c>
+      <c r="B10" t="s">
+        <v>575</v>
+      </c>
+      <c r="C10" t="s">
+        <v>509</v>
+      </c>
+      <c r="D10">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>577</v>
+      </c>
+      <c r="B11" t="s">
+        <v>445</v>
+      </c>
+      <c r="C11" t="s">
+        <v>444</v>
+      </c>
+      <c r="D11">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>578</v>
+      </c>
+      <c r="G11" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>580</v>
+      </c>
+      <c r="B12" t="s">
+        <v>440</v>
+      </c>
+      <c r="C12" t="s">
+        <v>439</v>
+      </c>
+      <c r="D12">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>581</v>
+      </c>
+      <c r="G12" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>583</v>
+      </c>
+      <c r="B13" t="s">
+        <v>447</v>
+      </c>
+      <c r="C13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D13">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>581</v>
+      </c>
+      <c r="G13" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>585</v>
+      </c>
+      <c r="B14" t="s">
+        <v>436</v>
+      </c>
+      <c r="C14" t="s">
+        <v>438</v>
+      </c>
+      <c r="D14">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>586</v>
+      </c>
+      <c r="G14" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>588</v>
+      </c>
+      <c r="B15" t="s">
+        <v>436</v>
+      </c>
+      <c r="C15" t="s">
+        <v>435</v>
+      </c>
+      <c r="D15">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>589</v>
+      </c>
+      <c r="G15" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>591</v>
+      </c>
+      <c r="B16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C16" t="s">
+        <v>454</v>
+      </c>
+      <c r="D16">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>592</v>
+      </c>
+      <c r="G16" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>594</v>
+      </c>
+      <c r="B17" t="s">
+        <v>436</v>
+      </c>
+      <c r="C17" t="s">
+        <v>450</v>
+      </c>
+      <c r="D17">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>595</v>
+      </c>
+      <c r="G17" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>597</v>
+      </c>
+      <c r="B18" t="s">
+        <v>436</v>
+      </c>
+      <c r="C18" t="s">
+        <v>451</v>
+      </c>
+      <c r="D18">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>598</v>
+      </c>
+      <c r="G18" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>600</v>
+      </c>
+      <c r="B19" t="s">
+        <v>436</v>
+      </c>
+      <c r="C19" t="s">
+        <v>448</v>
+      </c>
+      <c r="D19">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>601</v>
+      </c>
+      <c r="G19" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>603</v>
+      </c>
+      <c r="B20" t="s">
+        <v>436</v>
+      </c>
+      <c r="C20" t="s">
+        <v>449</v>
+      </c>
+      <c r="D20">
+        <v>32</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>589</v>
+      </c>
+      <c r="G20" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>605</v>
+      </c>
+      <c r="B21" t="s">
+        <v>606</v>
+      </c>
+      <c r="C21" t="s">
+        <v>501</v>
+      </c>
+      <c r="D21">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>608</v>
+      </c>
+      <c r="B22" t="s">
+        <v>434</v>
+      </c>
+      <c r="C22" t="s">
+        <v>433</v>
+      </c>
+      <c r="D22">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>586</v>
+      </c>
+      <c r="G22" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>610</v>
+      </c>
+      <c r="B23" t="s">
+        <v>434</v>
+      </c>
+      <c r="C23" t="s">
+        <v>437</v>
+      </c>
+      <c r="D23">
+        <v>32</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>589</v>
+      </c>
+      <c r="G23" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>612</v>
+      </c>
+      <c r="B24" t="s">
+        <v>434</v>
+      </c>
+      <c r="C24" t="s">
+        <v>460</v>
+      </c>
+      <c r="D24">
+        <v>32</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>592</v>
+      </c>
+      <c r="G24" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>614</v>
+      </c>
+      <c r="B25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C25" t="s">
+        <v>457</v>
+      </c>
+      <c r="D25">
+        <v>32</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>595</v>
+      </c>
+      <c r="G25" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>616</v>
+      </c>
+      <c r="B26" t="s">
+        <v>434</v>
+      </c>
+      <c r="C26" t="s">
+        <v>456</v>
+      </c>
+      <c r="D26">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>598</v>
+      </c>
+      <c r="G26" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>618</v>
+      </c>
+      <c r="B27" t="s">
+        <v>434</v>
+      </c>
+      <c r="C27" t="s">
+        <v>459</v>
+      </c>
+      <c r="D27">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>601</v>
+      </c>
+      <c r="G27" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>620</v>
+      </c>
+      <c r="B28" t="s">
+        <v>434</v>
+      </c>
+      <c r="C28" t="s">
+        <v>458</v>
+      </c>
+      <c r="D28">
+        <v>32</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>589</v>
+      </c>
+      <c r="G28" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>622</v>
+      </c>
+      <c r="B29" t="s">
+        <v>554</v>
+      </c>
+      <c r="C29" t="s">
+        <v>487</v>
+      </c>
+      <c r="D29">
+        <v>32</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>555</v>
+      </c>
+      <c r="G29" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>623</v>
+      </c>
+      <c r="B30" t="s">
+        <v>554</v>
+      </c>
+      <c r="C30" t="s">
+        <v>496</v>
+      </c>
+      <c r="D30">
+        <v>32</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>555</v>
+      </c>
+      <c r="G30" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>624</v>
+      </c>
+      <c r="B31" t="s">
+        <v>559</v>
+      </c>
+      <c r="C31" t="s">
+        <v>472</v>
+      </c>
+      <c r="D31">
+        <v>32</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>625</v>
+      </c>
+      <c r="B32" t="s">
+        <v>562</v>
+      </c>
+      <c r="C32" t="s">
+        <v>461</v>
+      </c>
+      <c r="D32">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>626</v>
+      </c>
+      <c r="B33" t="s">
+        <v>442</v>
+      </c>
+      <c r="C33" t="s">
+        <v>443</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>627</v>
+      </c>
+      <c r="B34" t="s">
+        <v>442</v>
+      </c>
+      <c r="C34" t="s">
+        <v>441</v>
+      </c>
+      <c r="D34">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>628</v>
+      </c>
+      <c r="B35" t="s">
+        <v>568</v>
+      </c>
+      <c r="C35" t="s">
+        <v>455</v>
+      </c>
+      <c r="D35">
+        <v>32</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>629</v>
+      </c>
+      <c r="B36" t="s">
+        <v>568</v>
+      </c>
+      <c r="C36" t="s">
+        <v>452</v>
+      </c>
+      <c r="D36">
+        <v>32</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>630</v>
+      </c>
+      <c r="B37" t="s">
+        <v>572</v>
+      </c>
+      <c r="C37" t="s">
+        <v>521</v>
+      </c>
+      <c r="D37">
+        <v>32</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>631</v>
+      </c>
+      <c r="B38" t="s">
+        <v>575</v>
+      </c>
+      <c r="C38" t="s">
+        <v>509</v>
+      </c>
+      <c r="D38">
+        <v>32</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>632</v>
+      </c>
+      <c r="B39" t="s">
+        <v>445</v>
+      </c>
+      <c r="C39" t="s">
+        <v>444</v>
+      </c>
+      <c r="D39">
+        <v>32</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>578</v>
+      </c>
+      <c r="G39" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>633</v>
+      </c>
+      <c r="B40" t="s">
+        <v>440</v>
+      </c>
+      <c r="C40" t="s">
+        <v>439</v>
+      </c>
+      <c r="D40">
+        <v>32</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>581</v>
+      </c>
+      <c r="G40" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>634</v>
+      </c>
+      <c r="B41" t="s">
+        <v>447</v>
+      </c>
+      <c r="C41" t="s">
+        <v>446</v>
+      </c>
+      <c r="D41">
+        <v>32</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>581</v>
+      </c>
+      <c r="G41" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>635</v>
+      </c>
+      <c r="B42" t="s">
+        <v>436</v>
+      </c>
+      <c r="C42" t="s">
+        <v>438</v>
+      </c>
+      <c r="D42">
+        <v>32</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>586</v>
+      </c>
+      <c r="G42" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>636</v>
+      </c>
+      <c r="B43" t="s">
+        <v>436</v>
+      </c>
+      <c r="C43" t="s">
+        <v>435</v>
+      </c>
+      <c r="D43">
+        <v>32</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>589</v>
+      </c>
+      <c r="G43" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>637</v>
+      </c>
+      <c r="B44" t="s">
+        <v>436</v>
+      </c>
+      <c r="C44" t="s">
+        <v>454</v>
+      </c>
+      <c r="D44">
+        <v>32</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>592</v>
+      </c>
+      <c r="G44" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>638</v>
+      </c>
+      <c r="B45" t="s">
+        <v>436</v>
+      </c>
+      <c r="C45" t="s">
+        <v>450</v>
+      </c>
+      <c r="D45">
+        <v>32</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>595</v>
+      </c>
+      <c r="G45" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>639</v>
+      </c>
+      <c r="B46" t="s">
+        <v>436</v>
+      </c>
+      <c r="C46" t="s">
+        <v>451</v>
+      </c>
+      <c r="D46">
+        <v>32</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>598</v>
+      </c>
+      <c r="G46" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>640</v>
+      </c>
+      <c r="B47" t="s">
+        <v>436</v>
+      </c>
+      <c r="C47" t="s">
+        <v>448</v>
+      </c>
+      <c r="D47">
+        <v>32</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>601</v>
+      </c>
+      <c r="G47" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>641</v>
+      </c>
+      <c r="B48" t="s">
+        <v>436</v>
+      </c>
+      <c r="C48" t="s">
+        <v>449</v>
+      </c>
+      <c r="D48">
+        <v>32</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>589</v>
+      </c>
+      <c r="G48" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>642</v>
+      </c>
+      <c r="B49" t="s">
+        <v>606</v>
+      </c>
+      <c r="C49" t="s">
+        <v>501</v>
+      </c>
+      <c r="D49">
+        <v>32</v>
+      </c>
+      <c r="E49" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>643</v>
+      </c>
+      <c r="B50" t="s">
+        <v>434</v>
+      </c>
+      <c r="C50" t="s">
+        <v>433</v>
+      </c>
+      <c r="D50">
+        <v>32</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>586</v>
+      </c>
+      <c r="G50" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>644</v>
+      </c>
+      <c r="B51" t="s">
+        <v>434</v>
+      </c>
+      <c r="C51" t="s">
+        <v>437</v>
+      </c>
+      <c r="D51">
+        <v>32</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>589</v>
+      </c>
+      <c r="G51" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>645</v>
+      </c>
+      <c r="B52" t="s">
+        <v>434</v>
+      </c>
+      <c r="C52" t="s">
+        <v>460</v>
+      </c>
+      <c r="D52">
+        <v>32</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>592</v>
+      </c>
+      <c r="G52" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>646</v>
+      </c>
+      <c r="B53" t="s">
+        <v>434</v>
+      </c>
+      <c r="C53" t="s">
+        <v>457</v>
+      </c>
+      <c r="D53">
+        <v>32</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>595</v>
+      </c>
+      <c r="G53" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>647</v>
+      </c>
+      <c r="B54" t="s">
+        <v>434</v>
+      </c>
+      <c r="C54" t="s">
+        <v>456</v>
+      </c>
+      <c r="D54">
+        <v>32</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>598</v>
+      </c>
+      <c r="G54" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>648</v>
+      </c>
+      <c r="B55" t="s">
+        <v>434</v>
+      </c>
+      <c r="C55" t="s">
+        <v>459</v>
+      </c>
+      <c r="D55">
+        <v>32</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>601</v>
+      </c>
+      <c r="G55" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>649</v>
+      </c>
+      <c r="B56" t="s">
+        <v>434</v>
+      </c>
+      <c r="C56" t="s">
+        <v>458</v>
+      </c>
+      <c r="D56">
+        <v>32</v>
+      </c>
+      <c r="E56" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>589</v>
+      </c>
+      <c r="G56" t="s">
+        <v>621</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{FB44FD47-0B92-4391-9CB5-FFD8B50F36C3}">
+      <selection activeCell="C9" sqref="C9"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>